<commit_message>
Remove unnecessary code for scatter chart
</commit_message>
<xml_diff>
--- a/Sandbox.OpenXML/ScatterChart.xlsx
+++ b/Sandbox.OpenXML/ScatterChart.xlsx
@@ -158,20 +158,9 @@
 </file>
 
 <file path=xl/drawings/charts/chart.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -550,14 +539,6 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:axId val="375001568"/>
         <c:axId val="375001960"/>
       </c:scatterChart>
@@ -567,7 +548,6 @@
           <c:orientation val="minMax"/>
           <c:max val="1"/>
         </c:scaling>
-        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -646,7 +626,6 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -759,37 +738,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="bg2"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins l="0.7" r="0.7" t="0.75" b="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1353,9 +1302,9 @@
 <xdr:wsDr xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>

</xml_diff>

<commit_message>
Remove unnecessary code for scatter matrix chart
</commit_message>
<xml_diff>
--- a/Sandbox.OpenXML/ScatterChart.xlsx
+++ b/Sandbox.OpenXML/ScatterChart.xlsx
@@ -24,30 +24,6 @@
     </x:ext>
   </x:extLst>
 </x:workbook>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<x:connections xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:connection id="1" name="Multivariate Data" type="6" refreshedVersion="5" background="1" saveData="1">
-    <x:textPr codePage="437" sourceFile="C:\Users\josueg\Documents\Projects\Deloitte\STAR Modernization - Magenic Documents\Multivariate Data.txt">
-      <x:textFields count="13">
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-        <x:textField/>
-      </x:textFields>
-    </x:textPr>
-  </x:connection>
-</x:connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -742,562 +718,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/charts/colors.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/drawings/charts/style.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1333,271 +753,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/queryTables/queryTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:queryTable xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Multivariate Data" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <x:dimension ref="A1:C47"/>

</xml_diff>